<commit_message>
file modified and ready to push
</commit_message>
<xml_diff>
--- a/Hometown Scenario.xlsx
+++ b/Hometown Scenario.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094D2B1B-5D38-43C3-974A-43C50C1B3B5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Functional" sheetId="1" r:id="rId1"/>
@@ -18,51 +12,18 @@
     <sheet name="globalisation testing" sheetId="4" r:id="rId3"/>
     <sheet name="End to end " sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>CBT</author>
-  </authors>
-  <commentList>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>CBT:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="269">
   <si>
     <t>Sl no</t>
   </si>
@@ -1161,12 +1122,18 @@
   <si>
     <t>intenalisation</t>
   </si>
+  <si>
+    <t>Login/logkn</t>
+  </si>
+  <si>
+    <t>Login/login</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1196,19 +1163,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -1291,7 +1245,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1564,32 +1518,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="5" max="5" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.109375" customWidth="1"/>
-    <col min="7" max="13" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="7" max="13" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1627,7 +1581,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="90">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1663,12 +1617,12 @@
       </c>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="105">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>267</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
@@ -1699,12 +1653,12 @@
       </c>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="105">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>268</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>25</v>
@@ -1735,7 +1689,7 @@
       </c>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="75">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1771,7 +1725,7 @@
       </c>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="90">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1807,7 +1761,7 @@
       </c>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="90">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1843,7 +1797,7 @@
       </c>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="90">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1879,7 +1833,7 @@
       </c>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="75">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1915,7 +1869,7 @@
       </c>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="75">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1951,7 +1905,7 @@
       </c>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="75">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1987,7 +1941,7 @@
       </c>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="90">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2023,7 +1977,7 @@
       </c>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="90">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2059,7 +2013,7 @@
       </c>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="75">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2095,7 +2049,7 @@
       </c>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="75">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2131,7 +2085,7 @@
       </c>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="75">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2167,7 +2121,7 @@
       </c>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="75">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2203,7 +2157,7 @@
       </c>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="75">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2239,7 +2193,7 @@
       </c>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="75">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2275,7 +2229,7 @@
       </c>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="90">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2311,7 +2265,7 @@
       </c>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="75">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2354,25 +2308,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="21.5546875" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.44140625" customWidth="1"/>
-    <col min="11" max="11" width="14.5546875" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
     <col min="13" max="15" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="30">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2419,7 +2373,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="165">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2451,7 +2405,7 @@
       </c>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:15" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="135">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2483,7 +2437,7 @@
       </c>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:15" ht="144" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="150">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2515,7 +2469,7 @@
       </c>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:15" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="180">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2547,7 +2501,7 @@
       </c>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:15" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="180">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2579,7 +2533,7 @@
       </c>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="120">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2611,7 +2565,7 @@
       </c>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="105">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2643,7 +2597,7 @@
       </c>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:15" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="135">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2675,7 +2629,7 @@
       </c>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:15" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="135">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2707,7 +2661,7 @@
       </c>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="135">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2739,7 +2693,7 @@
       </c>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2753,7 +2707,7 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2767,7 +2721,7 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2781,7 +2735,7 @@
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2795,7 +2749,7 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2809,7 +2763,7 @@
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2823,7 +2777,7 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2837,7 +2791,7 @@
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2851,7 +2805,7 @@
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2865,7 +2819,7 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2879,7 +2833,7 @@
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2893,7 +2847,7 @@
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2907,7 +2861,7 @@
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2921,7 +2875,7 @@
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2935,7 +2889,7 @@
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2949,7 +2903,7 @@
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2963,7 +2917,7 @@
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2977,7 +2931,7 @@
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2994,31 +2948,30 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD9FBD3F-B2A1-4743-A593-FD7FB3807004}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" s="9" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>266</v>
       </c>
@@ -3030,30 +2983,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="B56" sqref="B52:B56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" customWidth="1"/>
-    <col min="5" max="5" width="26.33203125" customWidth="1"/>
-    <col min="6" max="6" width="53.5546875" customWidth="1"/>
-    <col min="7" max="7" width="24.109375" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1"/>
-    <col min="11" max="11" width="14.109375" customWidth="1"/>
-    <col min="12" max="12" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1"/>
+    <col min="6" max="6" width="53.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="30">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3100,7 +3053,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="330">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3132,7 +3085,7 @@
       </c>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:15" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="285">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3164,7 +3117,7 @@
       </c>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:15" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="345">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3196,7 +3149,7 @@
       </c>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:15" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="345">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3228,7 +3181,7 @@
       </c>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:15" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="300">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3260,7 +3213,7 @@
       </c>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:15" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="409.5">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3292,7 +3245,7 @@
       </c>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:15" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="409.5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3324,7 +3277,7 @@
       </c>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:15" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="330">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3356,7 +3309,7 @@
       </c>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:15" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="409.5">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3388,7 +3341,7 @@
       </c>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:15" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="409.5">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3420,7 +3373,7 @@
       </c>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:15" ht="216" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="240">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3452,7 +3405,7 @@
       </c>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:15" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="360">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3484,7 +3437,7 @@
       </c>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:15" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="315">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3516,7 +3469,7 @@
       </c>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:15" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="390">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3548,7 +3501,7 @@
       </c>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:15" ht="360" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="405">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3580,7 +3533,7 @@
       </c>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="360">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3612,7 +3565,7 @@
       </c>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="405">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3644,7 +3597,7 @@
       </c>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="345">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3676,7 +3629,7 @@
       </c>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="409.5" customHeight="1">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3708,7 +3661,7 @@
       </c>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="409.5">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3740,7 +3693,7 @@
       </c>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="409.5">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3770,7 +3723,7 @@
       </c>
       <c r="L22" s="4"/>
     </row>
-    <row r="23" spans="1:12" ht="388.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="409.5">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3802,7 +3755,7 @@
       </c>
       <c r="L23" s="4"/>
     </row>
-    <row r="24" spans="1:12" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="360">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3834,7 +3787,7 @@
       </c>
       <c r="L24" s="4"/>
     </row>
-    <row r="25" spans="1:12" ht="360" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="405">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3862,7 +3815,7 @@
       </c>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:12" ht="301.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="301.5" customHeight="1">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3890,7 +3843,7 @@
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="44.25" customHeight="1">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3920,7 +3873,7 @@
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -3936,7 +3889,7 @@
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -3950,7 +3903,7 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -3964,7 +3917,7 @@
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -3978,7 +3931,7 @@
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -3992,7 +3945,7 @@
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -4006,7 +3959,7 @@
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -4020,7 +3973,7 @@
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>

</xml_diff>